<commit_message>
Committing before I change the PWM table (to point the AMUX the right way)
git-svn-id: https://svn.media.mit.edu/r/biomech-ee/Code/flexsea_1_0@521 ca98db78-25f0-4961-890e-003d10304561
</commit_message>
<xml_diff>
--- a/execute/ref/pwm.xlsx
+++ b/execute/ref/pwm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3930" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Brushed" sheetId="1" r:id="rId1"/>
@@ -650,12 +650,6 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +706,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1022,17 +1022,17 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1589,19 +1589,19 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="38" t="s">
         <v>16</v>
       </c>
       <c r="G25" s="13"/>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,66 +1821,66 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="45" t="s">
+      <c r="P3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="41" t="s">
         <v>29</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="46" t="str">
+      <c r="B4" s="44" t="str">
         <f>DEC2HEX(1*H4+2*G4+4*F4+8*E4+16*D4)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="47">
         <v>0</v>
       </c>
       <c r="D4" s="25">
@@ -1895,7 +1895,7 @@
       <c r="G4" s="25">
         <v>0</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="46">
         <v>0</v>
       </c>
       <c r="I4" s="25">
@@ -1919,14 +1919,14 @@
       <c r="O4" s="25">
         <v>0</v>
       </c>
-      <c r="P4" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="49" t="str">
+      <c r="P4" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="47" t="str">
         <f>DEC2HEX(1*P4+2*O4+4*N4+8*M4+16*L4+32*K4+64*J4+128*I4)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="50" t="b">
+      <c r="R4" s="48" t="b">
         <f>OR(AND(K4,L4), AND(M4,N4), AND(O4,P4))</f>
         <v>0</v>
       </c>
@@ -1934,11 +1934,11 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="49" t="str">
+      <c r="B5" s="47" t="str">
         <f t="shared" ref="B5:B35" si="0">DEC2HEX(1*H5+2*G5+4*F5+8*E5+16*D5)</f>
         <v>1</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="47">
         <v>1</v>
       </c>
       <c r="D5" s="25">
@@ -1953,14 +1953,14 @@
       <c r="G5" s="25">
         <v>0</v>
       </c>
-      <c r="H5" s="48">
+      <c r="H5" s="46">
         <v>1</v>
       </c>
       <c r="I5" s="25">
         <v>1</v>
       </c>
       <c r="J5" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="25">
         <v>1</v>
@@ -1978,15 +1978,15 @@
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="48">
+      <c r="P5" s="46">
         <f>D5</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="49" t="str">
+      <c r="Q5" s="47" t="str">
         <f t="shared" ref="Q5:Q35" si="1">DEC2HEX(1*P5+2*O5+4*N5+8*M5+16*L5+32*K5+64*J5+128*I5)</f>
-        <v>E0</v>
-      </c>
-      <c r="R5" s="51" t="b">
+        <v>A0</v>
+      </c>
+      <c r="R5" s="49" t="b">
         <f t="shared" ref="R5:R35" si="2">OR(AND(K5,L5), AND(M5,N5), AND(O5,P5))</f>
         <v>0</v>
       </c>
@@ -1994,11 +1994,11 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="49" t="str">
+      <c r="B6" s="47" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="47">
         <v>2</v>
       </c>
       <c r="D6" s="25">
@@ -2013,14 +2013,14 @@
       <c r="G6" s="25">
         <v>1</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="46">
         <v>0</v>
       </c>
       <c r="I6" s="25">
         <v>0</v>
       </c>
       <c r="J6" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="25">
         <v>0</v>
@@ -2039,14 +2039,14 @@
       <c r="O6" s="25">
         <v>1</v>
       </c>
-      <c r="P6" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="49" t="str">
+      <c r="P6" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="R6" s="51" t="b">
+        <v>2</v>
+      </c>
+      <c r="R6" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2054,11 +2054,11 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="49" t="str">
+      <c r="B7" s="47" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="47">
         <v>3</v>
       </c>
       <c r="D7" s="25">
@@ -2073,14 +2073,14 @@
       <c r="G7" s="25">
         <v>1</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="46">
         <v>1</v>
       </c>
       <c r="I7" s="25">
         <v>1</v>
       </c>
       <c r="J7" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="25">
         <v>1</v>
@@ -2099,14 +2099,14 @@
       <c r="O7" s="25">
         <v>0</v>
       </c>
-      <c r="P7" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="49" t="str">
+      <c r="P7" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>E0</v>
-      </c>
-      <c r="R7" s="51" t="b">
+        <v>A0</v>
+      </c>
+      <c r="R7" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2114,11 +2114,11 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="49" t="str">
+      <c r="B8" s="47" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="47">
         <v>4</v>
       </c>
       <c r="D8" s="25">
@@ -2133,14 +2133,14 @@
       <c r="G8" s="25">
         <v>0</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8" s="46">
         <v>0</v>
       </c>
       <c r="I8" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="25">
         <f>E8</f>
@@ -2159,14 +2159,14 @@
       <c r="O8" s="25">
         <v>0</v>
       </c>
-      <c r="P8" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="49" t="str">
+      <c r="P8" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="R8" s="51" t="b">
+        <v>48</v>
+      </c>
+      <c r="R8" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2174,11 +2174,11 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="49" t="str">
+      <c r="B9" s="47" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="47">
         <v>5</v>
       </c>
       <c r="D9" s="25">
@@ -2193,14 +2193,14 @@
       <c r="G9" s="25">
         <v>0</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9" s="46">
         <v>1</v>
       </c>
       <c r="I9" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="25">
         <v>0</v>
@@ -2218,15 +2218,15 @@
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="P9" s="48">
+      <c r="P9" s="46">
         <f>D9</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="49" t="str">
+      <c r="Q9" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="R9" s="51" t="b">
+        <v>48</v>
+      </c>
+      <c r="R9" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2234,11 +2234,11 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="49" t="str">
+      <c r="B10" s="47" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="47">
         <v>6</v>
       </c>
       <c r="D10" s="25">
@@ -2253,14 +2253,14 @@
       <c r="G10" s="25">
         <v>1</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="46">
         <v>0</v>
       </c>
       <c r="I10" s="25">
         <v>0</v>
       </c>
       <c r="J10" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="25">
         <f>E10</f>
@@ -2279,14 +2279,14 @@
       <c r="O10" s="25">
         <v>1</v>
       </c>
-      <c r="P10" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="49" t="str">
+      <c r="P10" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="R10" s="51" t="b">
+        <v>2</v>
+      </c>
+      <c r="R10" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2294,57 +2294,57 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="52" t="str">
+      <c r="B11" s="50" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="50">
         <v>7</v>
       </c>
-      <c r="D11" s="54">
-        <v>0</v>
-      </c>
-      <c r="E11" s="54">
-        <v>0</v>
-      </c>
-      <c r="F11" s="54">
-        <v>1</v>
-      </c>
-      <c r="G11" s="54">
-        <v>1</v>
-      </c>
-      <c r="H11" s="55">
-        <v>1</v>
-      </c>
-      <c r="I11" s="54">
-        <v>0</v>
-      </c>
-      <c r="J11" s="54">
-        <v>0</v>
-      </c>
-      <c r="K11" s="54">
-        <v>0</v>
-      </c>
-      <c r="L11" s="54">
-        <v>0</v>
-      </c>
-      <c r="M11" s="54">
-        <v>0</v>
-      </c>
-      <c r="N11" s="54">
-        <v>0</v>
-      </c>
-      <c r="O11" s="54">
-        <v>0</v>
-      </c>
-      <c r="P11" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="52" t="str">
+      <c r="D11" s="52">
+        <v>0</v>
+      </c>
+      <c r="E11" s="52">
+        <v>0</v>
+      </c>
+      <c r="F11" s="52">
+        <v>1</v>
+      </c>
+      <c r="G11" s="52">
+        <v>1</v>
+      </c>
+      <c r="H11" s="53">
+        <v>1</v>
+      </c>
+      <c r="I11" s="52">
+        <v>0</v>
+      </c>
+      <c r="J11" s="52">
+        <v>0</v>
+      </c>
+      <c r="K11" s="52">
+        <v>0</v>
+      </c>
+      <c r="L11" s="52">
+        <v>0</v>
+      </c>
+      <c r="M11" s="52">
+        <v>0</v>
+      </c>
+      <c r="N11" s="52">
+        <v>0</v>
+      </c>
+      <c r="O11" s="52">
+        <v>0</v>
+      </c>
+      <c r="P11" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="50" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R11" s="56" t="b">
+      <c r="R11" s="54" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2352,57 +2352,57 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="49" t="str">
+      <c r="B12" s="47" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C12" s="46">
-        <v>0</v>
-      </c>
-      <c r="D12" s="58">
+      <c r="C12" s="44">
+        <v>0</v>
+      </c>
+      <c r="D12" s="56">
         <v>0</v>
       </c>
       <c r="E12" s="25">
         <v>1</v>
       </c>
-      <c r="F12" s="58">
-        <v>0</v>
-      </c>
-      <c r="G12" s="58">
-        <v>0</v>
-      </c>
-      <c r="H12" s="59">
-        <v>0</v>
-      </c>
-      <c r="I12" s="58">
-        <v>0</v>
-      </c>
-      <c r="J12" s="58">
-        <v>0</v>
-      </c>
-      <c r="K12" s="58">
-        <v>0</v>
-      </c>
-      <c r="L12" s="58">
-        <v>0</v>
-      </c>
-      <c r="M12" s="58">
-        <v>0</v>
-      </c>
-      <c r="N12" s="58">
-        <v>0</v>
-      </c>
-      <c r="O12" s="58">
-        <v>0</v>
-      </c>
-      <c r="P12" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="49" t="str">
+      <c r="F12" s="56">
+        <v>0</v>
+      </c>
+      <c r="G12" s="56">
+        <v>0</v>
+      </c>
+      <c r="H12" s="57">
+        <v>0</v>
+      </c>
+      <c r="I12" s="56">
+        <v>0</v>
+      </c>
+      <c r="J12" s="56">
+        <v>0</v>
+      </c>
+      <c r="K12" s="56">
+        <v>0</v>
+      </c>
+      <c r="L12" s="56">
+        <v>0</v>
+      </c>
+      <c r="M12" s="56">
+        <v>0</v>
+      </c>
+      <c r="N12" s="56">
+        <v>0</v>
+      </c>
+      <c r="O12" s="56">
+        <v>0</v>
+      </c>
+      <c r="P12" s="57">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R12" s="51" t="b">
+      <c r="R12" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2410,11 +2410,11 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="49" t="str">
+      <c r="B13" s="47" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="47">
         <v>1</v>
       </c>
       <c r="D13" s="25">
@@ -2429,14 +2429,14 @@
       <c r="G13" s="25">
         <v>0</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="46">
         <v>1</v>
       </c>
       <c r="I13" s="25">
         <v>1</v>
       </c>
       <c r="J13" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="25">
         <v>1</v>
@@ -2454,15 +2454,15 @@
         <f>E13</f>
         <v>1</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="46">
         <f>D13</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="49" t="str">
+      <c r="Q13" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="R13" s="51" t="b">
+        <v>A2</v>
+      </c>
+      <c r="R13" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2470,11 +2470,11 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="49" t="str">
+      <c r="B14" s="47" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="47">
         <v>2</v>
       </c>
       <c r="D14" s="25">
@@ -2489,14 +2489,14 @@
       <c r="G14" s="25">
         <v>1</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14" s="46">
         <v>0</v>
       </c>
       <c r="I14" s="25">
         <v>0</v>
       </c>
       <c r="J14" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="25">
         <v>0</v>
@@ -2515,194 +2515,194 @@
       <c r="O14" s="25">
         <v>1</v>
       </c>
-      <c r="P14" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="49" t="str">
+      <c r="P14" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="R14" s="49" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="C15" s="47">
+        <v>3</v>
+      </c>
+      <c r="D15" s="25">
+        <v>0</v>
+      </c>
+      <c r="E15" s="25">
+        <v>1</v>
+      </c>
+      <c r="F15" s="25">
+        <v>0</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1</v>
+      </c>
+      <c r="H15" s="46">
+        <v>1</v>
+      </c>
+      <c r="I15" s="25">
+        <v>1</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25">
+        <v>1</v>
+      </c>
+      <c r="L15" s="25">
+        <v>0</v>
+      </c>
+      <c r="M15" s="25">
+        <f>E15</f>
+        <v>1</v>
+      </c>
+      <c r="N15" s="25">
+        <f>D15</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="25">
+        <v>0</v>
+      </c>
+      <c r="P15" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>A8</v>
+      </c>
+      <c r="R15" s="49" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="C16" s="47">
+        <v>4</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25">
+        <v>1</v>
+      </c>
+      <c r="F16" s="25">
+        <v>1</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0</v>
+      </c>
+      <c r="H16" s="46">
+        <v>0</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0</v>
+      </c>
+      <c r="J16" s="25">
+        <v>1</v>
+      </c>
+      <c r="K16" s="25">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="25">
+        <f>D16</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="25">
+        <v>1</v>
+      </c>
+      <c r="N16" s="25">
+        <v>0</v>
+      </c>
+      <c r="O16" s="25">
+        <v>0</v>
+      </c>
+      <c r="P16" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="R16" s="49" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="C17" s="47">
+        <v>5</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="46">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0</v>
+      </c>
+      <c r="J17" s="25">
+        <v>1</v>
+      </c>
+      <c r="K17" s="25">
+        <v>0</v>
+      </c>
+      <c r="L17" s="25">
+        <v>0</v>
+      </c>
+      <c r="M17" s="25">
+        <v>1</v>
+      </c>
+      <c r="N17" s="25">
+        <v>0</v>
+      </c>
+      <c r="O17" s="25">
+        <f>E17</f>
+        <v>1</v>
+      </c>
+      <c r="P17" s="46">
+        <f>D17</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="47" t="str">
         <f t="shared" si="1"/>
         <v>4A</v>
       </c>
-      <c r="R14" s="51" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>B</v>
-      </c>
-      <c r="C15" s="49">
-        <v>3</v>
-      </c>
-      <c r="D15" s="25">
-        <v>0</v>
-      </c>
-      <c r="E15" s="25">
-        <v>1</v>
-      </c>
-      <c r="F15" s="25">
-        <v>0</v>
-      </c>
-      <c r="G15" s="25">
-        <v>1</v>
-      </c>
-      <c r="H15" s="48">
-        <v>1</v>
-      </c>
-      <c r="I15" s="25">
-        <v>1</v>
-      </c>
-      <c r="J15" s="25">
-        <v>1</v>
-      </c>
-      <c r="K15" s="25">
-        <v>1</v>
-      </c>
-      <c r="L15" s="25">
-        <v>0</v>
-      </c>
-      <c r="M15" s="25">
-        <f>E15</f>
-        <v>1</v>
-      </c>
-      <c r="N15" s="25">
-        <f>D15</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="25">
-        <v>0</v>
-      </c>
-      <c r="P15" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="49" t="str">
-        <f t="shared" si="1"/>
-        <v>E8</v>
-      </c>
-      <c r="R15" s="51" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>C</v>
-      </c>
-      <c r="C16" s="49">
-        <v>4</v>
-      </c>
-      <c r="D16" s="25">
-        <v>0</v>
-      </c>
-      <c r="E16" s="25">
-        <v>1</v>
-      </c>
-      <c r="F16" s="25">
-        <v>1</v>
-      </c>
-      <c r="G16" s="25">
-        <v>0</v>
-      </c>
-      <c r="H16" s="48">
-        <v>0</v>
-      </c>
-      <c r="I16" s="25">
-        <v>1</v>
-      </c>
-      <c r="J16" s="25">
-        <v>0</v>
-      </c>
-      <c r="K16" s="25">
-        <f>E16</f>
-        <v>1</v>
-      </c>
-      <c r="L16" s="25">
-        <f>D16</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="25">
-        <v>1</v>
-      </c>
-      <c r="N16" s="25">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25">
-        <v>0</v>
-      </c>
-      <c r="P16" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="49" t="str">
-        <f t="shared" si="1"/>
-        <v>A8</v>
-      </c>
-      <c r="R16" s="51" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>D</v>
-      </c>
-      <c r="C17" s="49">
-        <v>5</v>
-      </c>
-      <c r="D17" s="25">
-        <v>0</v>
-      </c>
-      <c r="E17" s="25">
-        <v>1</v>
-      </c>
-      <c r="F17" s="25">
-        <v>1</v>
-      </c>
-      <c r="G17" s="25">
-        <v>0</v>
-      </c>
-      <c r="H17" s="48">
-        <v>1</v>
-      </c>
-      <c r="I17" s="25">
-        <v>1</v>
-      </c>
-      <c r="J17" s="25">
-        <v>0</v>
-      </c>
-      <c r="K17" s="25">
-        <v>0</v>
-      </c>
-      <c r="L17" s="25">
-        <v>0</v>
-      </c>
-      <c r="M17" s="25">
-        <v>1</v>
-      </c>
-      <c r="N17" s="25">
-        <v>0</v>
-      </c>
-      <c r="O17" s="25">
-        <f>E17</f>
-        <v>1</v>
-      </c>
-      <c r="P17" s="48">
-        <f>D17</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="49" t="str">
-        <f t="shared" si="1"/>
-        <v>8A</v>
-      </c>
-      <c r="R17" s="51" t="b">
+      <c r="R17" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2710,11 +2710,11 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="49" t="str">
+      <c r="B18" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="47">
         <v>6</v>
       </c>
       <c r="D18" s="25">
@@ -2729,14 +2729,14 @@
       <c r="G18" s="25">
         <v>1</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="46">
         <v>0</v>
       </c>
       <c r="I18" s="25">
         <v>0</v>
       </c>
       <c r="J18" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="25">
         <f>E18</f>
@@ -2755,14 +2755,14 @@
       <c r="O18" s="25">
         <v>1</v>
       </c>
-      <c r="P18" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="49" t="str">
+      <c r="P18" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="R18" s="51" t="b">
+        <v>22</v>
+      </c>
+      <c r="R18" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2770,57 +2770,57 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="49" t="str">
+      <c r="B19" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="50">
         <v>7</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="52">
         <v>0</v>
       </c>
       <c r="E19" s="25">
         <v>1</v>
       </c>
-      <c r="F19" s="54">
-        <v>1</v>
-      </c>
-      <c r="G19" s="54">
-        <v>1</v>
-      </c>
-      <c r="H19" s="55">
-        <v>1</v>
-      </c>
-      <c r="I19" s="54">
-        <v>0</v>
-      </c>
-      <c r="J19" s="54">
-        <v>0</v>
-      </c>
-      <c r="K19" s="54">
-        <v>0</v>
-      </c>
-      <c r="L19" s="54">
-        <v>0</v>
-      </c>
-      <c r="M19" s="54">
-        <v>0</v>
-      </c>
-      <c r="N19" s="54">
-        <v>0</v>
-      </c>
-      <c r="O19" s="54">
-        <v>0</v>
-      </c>
-      <c r="P19" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="49" t="str">
+      <c r="F19" s="52">
+        <v>1</v>
+      </c>
+      <c r="G19" s="52">
+        <v>1</v>
+      </c>
+      <c r="H19" s="53">
+        <v>1</v>
+      </c>
+      <c r="I19" s="52">
+        <v>0</v>
+      </c>
+      <c r="J19" s="52">
+        <v>0</v>
+      </c>
+      <c r="K19" s="52">
+        <v>0</v>
+      </c>
+      <c r="L19" s="52">
+        <v>0</v>
+      </c>
+      <c r="M19" s="52">
+        <v>0</v>
+      </c>
+      <c r="N19" s="52">
+        <v>0</v>
+      </c>
+      <c r="O19" s="52">
+        <v>0</v>
+      </c>
+      <c r="P19" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R19" s="51" t="b">
+      <c r="R19" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2828,57 +2828,57 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="46" t="str">
+      <c r="B20" s="44" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C20" s="46">
-        <v>0</v>
-      </c>
-      <c r="D20" s="58">
-        <v>1</v>
-      </c>
-      <c r="E20" s="58">
-        <v>0</v>
-      </c>
-      <c r="F20" s="58">
-        <v>0</v>
-      </c>
-      <c r="G20" s="58">
-        <v>0</v>
-      </c>
-      <c r="H20" s="59">
-        <v>0</v>
-      </c>
-      <c r="I20" s="58">
-        <v>0</v>
-      </c>
-      <c r="J20" s="58">
-        <v>0</v>
-      </c>
-      <c r="K20" s="58">
-        <v>0</v>
-      </c>
-      <c r="L20" s="58">
-        <v>0</v>
-      </c>
-      <c r="M20" s="58">
-        <v>0</v>
-      </c>
-      <c r="N20" s="58">
-        <v>0</v>
-      </c>
-      <c r="O20" s="58">
-        <v>0</v>
-      </c>
-      <c r="P20" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="46" t="str">
+      <c r="C20" s="44">
+        <v>0</v>
+      </c>
+      <c r="D20" s="56">
+        <v>1</v>
+      </c>
+      <c r="E20" s="56">
+        <v>0</v>
+      </c>
+      <c r="F20" s="56">
+        <v>0</v>
+      </c>
+      <c r="G20" s="56">
+        <v>0</v>
+      </c>
+      <c r="H20" s="57">
+        <v>0</v>
+      </c>
+      <c r="I20" s="56">
+        <v>0</v>
+      </c>
+      <c r="J20" s="56">
+        <v>0</v>
+      </c>
+      <c r="K20" s="56">
+        <v>0</v>
+      </c>
+      <c r="L20" s="56">
+        <v>0</v>
+      </c>
+      <c r="M20" s="56">
+        <v>0</v>
+      </c>
+      <c r="N20" s="56">
+        <v>0</v>
+      </c>
+      <c r="O20" s="56">
+        <v>0</v>
+      </c>
+      <c r="P20" s="57">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="44" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R20" s="50" t="b">
+      <c r="R20" s="48" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2886,11 +2886,11 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="49" t="str">
+      <c r="B21" s="47" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="47">
         <v>1</v>
       </c>
       <c r="D21" s="25">
@@ -2905,14 +2905,14 @@
       <c r="G21" s="25">
         <v>0</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="46">
         <v>1</v>
       </c>
       <c r="I21" s="25">
         <v>1</v>
       </c>
       <c r="J21" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="25">
         <v>1</v>
@@ -2930,15 +2930,15 @@
         <f>E21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="48">
+      <c r="P21" s="46">
         <f>D21</f>
         <v>1</v>
       </c>
-      <c r="Q21" s="49" t="str">
+      <c r="Q21" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>E1</v>
-      </c>
-      <c r="R21" s="51" t="b">
+        <v>A1</v>
+      </c>
+      <c r="R21" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2946,11 +2946,11 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="49" t="str">
+      <c r="B22" s="47" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="47">
         <v>2</v>
       </c>
       <c r="D22" s="25">
@@ -2965,14 +2965,14 @@
       <c r="G22" s="25">
         <v>1</v>
       </c>
-      <c r="H22" s="48">
+      <c r="H22" s="46">
         <v>0</v>
       </c>
       <c r="I22" s="25">
         <v>0</v>
       </c>
       <c r="J22" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="25">
         <v>0</v>
@@ -2991,14 +2991,14 @@
       <c r="O22" s="25">
         <v>1</v>
       </c>
-      <c r="P22" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="49" t="str">
+      <c r="P22" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="R22" s="51" t="b">
+        <v>6</v>
+      </c>
+      <c r="R22" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3006,11 +3006,11 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="49" t="str">
+      <c r="B23" s="47" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="47">
         <v>3</v>
       </c>
       <c r="D23" s="25">
@@ -3025,14 +3025,14 @@
       <c r="G23" s="25">
         <v>1</v>
       </c>
-      <c r="H23" s="48">
+      <c r="H23" s="46">
         <v>1</v>
       </c>
       <c r="I23" s="25">
         <v>1</v>
       </c>
       <c r="J23" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="25">
         <v>1</v>
@@ -3051,14 +3051,14 @@
       <c r="O23" s="25">
         <v>0</v>
       </c>
-      <c r="P23" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="49" t="str">
+      <c r="P23" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="R23" s="51" t="b">
+        <v>A4</v>
+      </c>
+      <c r="R23" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3066,11 +3066,11 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="49" t="str">
+      <c r="B24" s="47" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="47">
         <v>4</v>
       </c>
       <c r="D24" s="25">
@@ -3085,14 +3085,14 @@
       <c r="G24" s="25">
         <v>0</v>
       </c>
-      <c r="H24" s="48">
+      <c r="H24" s="46">
         <v>0</v>
       </c>
       <c r="I24" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="25">
         <f>E24</f>
@@ -3111,14 +3111,14 @@
       <c r="O24" s="25">
         <v>0</v>
       </c>
-      <c r="P24" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="49" t="str">
+      <c r="P24" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="R24" s="51" t="b">
+        <v>58</v>
+      </c>
+      <c r="R24" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3126,11 +3126,11 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="49" t="str">
+      <c r="B25" s="47" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25" s="47">
         <v>5</v>
       </c>
       <c r="D25" s="25">
@@ -3145,14 +3145,14 @@
       <c r="G25" s="25">
         <v>0</v>
       </c>
-      <c r="H25" s="48">
+      <c r="H25" s="46">
         <v>1</v>
       </c>
       <c r="I25" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="25">
         <v>0</v>
@@ -3170,15 +3170,15 @@
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="P25" s="48">
+      <c r="P25" s="46">
         <f>D25</f>
         <v>1</v>
       </c>
-      <c r="Q25" s="49" t="str">
+      <c r="Q25" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="R25" s="51" t="b">
+        <v>49</v>
+      </c>
+      <c r="R25" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3186,11 +3186,11 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="49" t="str">
+      <c r="B26" s="47" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="47">
         <v>6</v>
       </c>
       <c r="D26" s="25">
@@ -3205,14 +3205,14 @@
       <c r="G26" s="25">
         <v>1</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="46">
         <v>0</v>
       </c>
       <c r="I26" s="25">
         <v>0</v>
       </c>
       <c r="J26" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="25">
         <f>E26</f>
@@ -3231,14 +3231,14 @@
       <c r="O26" s="25">
         <v>1</v>
       </c>
-      <c r="P26" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="49" t="str">
+      <c r="P26" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="47" t="str">
         <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="R26" s="51" t="b">
+        <v>12</v>
+      </c>
+      <c r="R26" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3246,57 +3246,57 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="52" t="str">
+      <c r="B27" s="50" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="50">
         <v>7</v>
       </c>
-      <c r="D27" s="54">
-        <v>1</v>
-      </c>
-      <c r="E27" s="54">
-        <v>0</v>
-      </c>
-      <c r="F27" s="54">
-        <v>1</v>
-      </c>
-      <c r="G27" s="54">
-        <v>1</v>
-      </c>
-      <c r="H27" s="55">
-        <v>1</v>
-      </c>
-      <c r="I27" s="54">
-        <v>0</v>
-      </c>
-      <c r="J27" s="54">
-        <v>0</v>
-      </c>
-      <c r="K27" s="54">
-        <v>0</v>
-      </c>
-      <c r="L27" s="54">
-        <v>0</v>
-      </c>
-      <c r="M27" s="54">
-        <v>0</v>
-      </c>
-      <c r="N27" s="54">
-        <v>0</v>
-      </c>
-      <c r="O27" s="54">
-        <v>0</v>
-      </c>
-      <c r="P27" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="52" t="str">
+      <c r="D27" s="52">
+        <v>1</v>
+      </c>
+      <c r="E27" s="52">
+        <v>0</v>
+      </c>
+      <c r="F27" s="52">
+        <v>1</v>
+      </c>
+      <c r="G27" s="52">
+        <v>1</v>
+      </c>
+      <c r="H27" s="53">
+        <v>1</v>
+      </c>
+      <c r="I27" s="52">
+        <v>0</v>
+      </c>
+      <c r="J27" s="52">
+        <v>0</v>
+      </c>
+      <c r="K27" s="52">
+        <v>0</v>
+      </c>
+      <c r="L27" s="52">
+        <v>0</v>
+      </c>
+      <c r="M27" s="52">
+        <v>0</v>
+      </c>
+      <c r="N27" s="52">
+        <v>0</v>
+      </c>
+      <c r="O27" s="52">
+        <v>0</v>
+      </c>
+      <c r="P27" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="50" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R27" s="56" t="b">
+      <c r="R27" s="54" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3304,11 +3304,11 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="46" t="str">
+      <c r="B28" s="44" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="47">
         <v>0</v>
       </c>
       <c r="D28" s="25">
@@ -3323,38 +3323,38 @@
       <c r="G28" s="25">
         <v>0</v>
       </c>
-      <c r="H28" s="48">
-        <v>0</v>
-      </c>
-      <c r="I28" s="57">
-        <v>0</v>
-      </c>
-      <c r="J28" s="58">
-        <v>0</v>
-      </c>
-      <c r="K28" s="58">
-        <v>0</v>
-      </c>
-      <c r="L28" s="58">
-        <v>0</v>
-      </c>
-      <c r="M28" s="58">
-        <v>0</v>
-      </c>
-      <c r="N28" s="58">
-        <v>0</v>
-      </c>
-      <c r="O28" s="58">
-        <v>0</v>
-      </c>
-      <c r="P28" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="49" t="str">
+      <c r="H28" s="46">
+        <v>0</v>
+      </c>
+      <c r="I28" s="55">
+        <v>0</v>
+      </c>
+      <c r="J28" s="56">
+        <v>0</v>
+      </c>
+      <c r="K28" s="56">
+        <v>0</v>
+      </c>
+      <c r="L28" s="56">
+        <v>0</v>
+      </c>
+      <c r="M28" s="56">
+        <v>0</v>
+      </c>
+      <c r="N28" s="56">
+        <v>0</v>
+      </c>
+      <c r="O28" s="56">
+        <v>0</v>
+      </c>
+      <c r="P28" s="57">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R28" s="51" t="b">
+      <c r="R28" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3362,11 +3362,11 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="49" t="str">
+      <c r="B29" s="47" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C29" s="49">
+      <c r="C29" s="47">
         <v>1</v>
       </c>
       <c r="D29" s="25">
@@ -3381,10 +3381,10 @@
       <c r="G29" s="25">
         <v>0</v>
       </c>
-      <c r="H29" s="48">
-        <v>1</v>
-      </c>
-      <c r="I29" s="47">
+      <c r="H29" s="46">
+        <v>1</v>
+      </c>
+      <c r="I29" s="45">
         <v>0</v>
       </c>
       <c r="J29" s="25">
@@ -3405,14 +3405,14 @@
       <c r="O29" s="25">
         <v>0</v>
       </c>
-      <c r="P29" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="49" t="str">
+      <c r="P29" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R29" s="51" t="b">
+      <c r="R29" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3420,11 +3420,11 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="49" t="str">
+      <c r="B30" s="47" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="C30" s="49">
+      <c r="C30" s="47">
         <v>2</v>
       </c>
       <c r="D30" s="25">
@@ -3439,10 +3439,10 @@
       <c r="G30" s="25">
         <v>1</v>
       </c>
-      <c r="H30" s="48">
-        <v>0</v>
-      </c>
-      <c r="I30" s="47">
+      <c r="H30" s="46">
+        <v>0</v>
+      </c>
+      <c r="I30" s="45">
         <v>0</v>
       </c>
       <c r="J30" s="25">
@@ -3463,14 +3463,14 @@
       <c r="O30" s="25">
         <v>0</v>
       </c>
-      <c r="P30" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="49" t="str">
+      <c r="P30" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R30" s="51" t="b">
+      <c r="R30" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3478,11 +3478,11 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="49" t="str">
+      <c r="B31" s="47" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="C31" s="49">
+      <c r="C31" s="47">
         <v>3</v>
       </c>
       <c r="D31" s="25">
@@ -3497,10 +3497,10 @@
       <c r="G31" s="25">
         <v>1</v>
       </c>
-      <c r="H31" s="48">
-        <v>1</v>
-      </c>
-      <c r="I31" s="47">
+      <c r="H31" s="46">
+        <v>1</v>
+      </c>
+      <c r="I31" s="45">
         <v>0</v>
       </c>
       <c r="J31" s="25">
@@ -3521,14 +3521,14 @@
       <c r="O31" s="25">
         <v>0</v>
       </c>
-      <c r="P31" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="49" t="str">
+      <c r="P31" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R31" s="51" t="b">
+      <c r="R31" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3536,11 +3536,11 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="49" t="str">
+      <c r="B32" s="47" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="C32" s="49">
+      <c r="C32" s="47">
         <v>4</v>
       </c>
       <c r="D32" s="25">
@@ -3555,10 +3555,10 @@
       <c r="G32" s="25">
         <v>0</v>
       </c>
-      <c r="H32" s="48">
-        <v>0</v>
-      </c>
-      <c r="I32" s="47">
+      <c r="H32" s="46">
+        <v>0</v>
+      </c>
+      <c r="I32" s="45">
         <v>0</v>
       </c>
       <c r="J32" s="25">
@@ -3579,14 +3579,14 @@
       <c r="O32" s="25">
         <v>0</v>
       </c>
-      <c r="P32" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="49" t="str">
+      <c r="P32" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R32" s="51" t="b">
+      <c r="R32" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3594,11 +3594,11 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="49" t="str">
+      <c r="B33" s="47" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="47">
         <v>5</v>
       </c>
       <c r="D33" s="25">
@@ -3613,10 +3613,10 @@
       <c r="G33" s="25">
         <v>0</v>
       </c>
-      <c r="H33" s="48">
-        <v>1</v>
-      </c>
-      <c r="I33" s="47">
+      <c r="H33" s="46">
+        <v>1</v>
+      </c>
+      <c r="I33" s="45">
         <v>0</v>
       </c>
       <c r="J33" s="25">
@@ -3637,14 +3637,14 @@
       <c r="O33" s="25">
         <v>0</v>
       </c>
-      <c r="P33" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="49" t="str">
+      <c r="P33" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R33" s="51" t="b">
+      <c r="R33" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3652,11 +3652,11 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="49" t="str">
+      <c r="B34" s="47" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="C34" s="49">
+      <c r="C34" s="47">
         <v>6</v>
       </c>
       <c r="D34" s="25">
@@ -3671,10 +3671,10 @@
       <c r="G34" s="25">
         <v>1</v>
       </c>
-      <c r="H34" s="48">
-        <v>0</v>
-      </c>
-      <c r="I34" s="47">
+      <c r="H34" s="46">
+        <v>0</v>
+      </c>
+      <c r="I34" s="45">
         <v>0</v>
       </c>
       <c r="J34" s="25">
@@ -3695,14 +3695,14 @@
       <c r="O34" s="25">
         <v>0</v>
       </c>
-      <c r="P34" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="49" t="str">
+      <c r="P34" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="47" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R34" s="51" t="b">
+      <c r="R34" s="49" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3710,57 +3710,57 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="52" t="str">
+      <c r="B35" s="50" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="C35" s="52">
+      <c r="C35" s="50">
         <v>7</v>
       </c>
-      <c r="D35" s="54">
-        <v>1</v>
-      </c>
-      <c r="E35" s="54">
-        <v>1</v>
-      </c>
-      <c r="F35" s="54">
-        <v>1</v>
-      </c>
-      <c r="G35" s="54">
-        <v>1</v>
-      </c>
-      <c r="H35" s="55">
-        <v>1</v>
-      </c>
-      <c r="I35" s="53">
-        <v>0</v>
-      </c>
-      <c r="J35" s="54">
-        <v>0</v>
-      </c>
-      <c r="K35" s="54">
-        <v>0</v>
-      </c>
-      <c r="L35" s="54">
-        <v>0</v>
-      </c>
-      <c r="M35" s="54">
-        <v>0</v>
-      </c>
-      <c r="N35" s="54">
-        <v>0</v>
-      </c>
-      <c r="O35" s="54">
-        <v>0</v>
-      </c>
-      <c r="P35" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="52" t="str">
+      <c r="D35" s="52">
+        <v>1</v>
+      </c>
+      <c r="E35" s="52">
+        <v>1</v>
+      </c>
+      <c r="F35" s="52">
+        <v>1</v>
+      </c>
+      <c r="G35" s="52">
+        <v>1</v>
+      </c>
+      <c r="H35" s="53">
+        <v>1</v>
+      </c>
+      <c r="I35" s="51">
+        <v>0</v>
+      </c>
+      <c r="J35" s="52">
+        <v>0</v>
+      </c>
+      <c r="K35" s="52">
+        <v>0</v>
+      </c>
+      <c r="L35" s="52">
+        <v>0</v>
+      </c>
+      <c r="M35" s="52">
+        <v>0</v>
+      </c>
+      <c r="N35" s="52">
+        <v>0</v>
+      </c>
+      <c r="O35" s="52">
+        <v>0</v>
+      </c>
+      <c r="P35" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="50" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R35" s="56" t="b">
+      <c r="R35" s="54" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3801,7 +3801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -3828,38 +3828,38 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="43" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="47" t="str">
         <f>DEC2HEX(1*F3+2*E3+4*D3+8*C3)</f>
         <v>0</v>
       </c>
@@ -3875,16 +3875,16 @@
       <c r="F3" s="25">
         <v>0</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="45">
         <v>0</v>
       </c>
       <c r="H3" s="25">
         <v>0</v>
       </c>
-      <c r="I3" s="48">
-        <v>0</v>
-      </c>
-      <c r="J3" s="48" t="str">
+      <c r="I3" s="46">
+        <v>0</v>
+      </c>
+      <c r="J3" s="46" t="str">
         <f>DEC2HEX(1*I3+2*H3+4*G3)</f>
         <v>0</v>
       </c>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="49" t="str">
+      <c r="B4" s="47" t="str">
         <f t="shared" ref="B4:B18" si="0">DEC2HEX(1*F4+2*E4+4*D4+8*C4)</f>
         <v>1</v>
       </c>
@@ -3908,16 +3908,16 @@
       <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="45">
         <v>0</v>
       </c>
       <c r="H4" s="25">
         <v>0</v>
       </c>
-      <c r="I4" s="48">
-        <v>1</v>
-      </c>
-      <c r="J4" s="48" t="str">
+      <c r="I4" s="46">
+        <v>1</v>
+      </c>
+      <c r="J4" s="46" t="str">
         <f t="shared" ref="J4:J18" si="1">DEC2HEX(1*I4+2*H4+4*G4)</f>
         <v>1</v>
       </c>
@@ -3925,7 +3925,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
-      <c r="B5" s="49" t="str">
+      <c r="B5" s="47" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3941,16 +3941,16 @@
       <c r="F5" s="25">
         <v>0</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="45">
         <v>0</v>
       </c>
       <c r="H5" s="25">
         <v>1</v>
       </c>
-      <c r="I5" s="48">
-        <v>0</v>
-      </c>
-      <c r="J5" s="48" t="str">
+      <c r="I5" s="46">
+        <v>0</v>
+      </c>
+      <c r="J5" s="46" t="str">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
-      <c r="B6" s="49" t="str">
+      <c r="B6" s="47" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -3974,16 +3974,16 @@
       <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="45">
         <v>0</v>
       </c>
       <c r="H6" s="25">
         <v>1</v>
       </c>
-      <c r="I6" s="48">
-        <v>1</v>
-      </c>
-      <c r="J6" s="48" t="str">
+      <c r="I6" s="46">
+        <v>1</v>
+      </c>
+      <c r="J6" s="46" t="str">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
-      <c r="B7" s="49" t="str">
+      <c r="B7" s="47" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -4007,16 +4007,16 @@
       <c r="F7" s="25">
         <v>0</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="45">
         <v>1</v>
       </c>
       <c r="H7" s="25">
         <v>0</v>
       </c>
-      <c r="I7" s="48">
-        <v>0</v>
-      </c>
-      <c r="J7" s="48" t="str">
+      <c r="I7" s="46">
+        <v>0</v>
+      </c>
+      <c r="J7" s="46" t="str">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
-      <c r="B8" s="49" t="str">
+      <c r="B8" s="47" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -4040,16 +4040,16 @@
       <c r="F8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="45">
         <v>1</v>
       </c>
       <c r="H8" s="25">
         <v>0</v>
       </c>
-      <c r="I8" s="48">
-        <v>1</v>
-      </c>
-      <c r="J8" s="48" t="str">
+      <c r="I8" s="46">
+        <v>1</v>
+      </c>
+      <c r="J8" s="46" t="str">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
-      <c r="B9" s="49" t="str">
+      <c r="B9" s="47" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4073,16 +4073,16 @@
       <c r="F9" s="25">
         <v>0</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="45">
         <v>1</v>
       </c>
       <c r="H9" s="25">
         <v>1</v>
       </c>
-      <c r="I9" s="48">
-        <v>0</v>
-      </c>
-      <c r="J9" s="48" t="str">
+      <c r="I9" s="46">
+        <v>0</v>
+      </c>
+      <c r="J9" s="46" t="str">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
-      <c r="B10" s="49" t="str">
+      <c r="B10" s="47" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -4106,16 +4106,16 @@
       <c r="F10" s="25">
         <v>1</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="45">
         <v>1</v>
       </c>
       <c r="H10" s="25">
         <v>1</v>
       </c>
-      <c r="I10" s="48">
-        <v>1</v>
-      </c>
-      <c r="J10" s="48" t="str">
+      <c r="I10" s="46">
+        <v>1</v>
+      </c>
+      <c r="J10" s="46" t="str">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -4123,32 +4123,32 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="46" t="str">
+      <c r="B11" s="44" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="58">
-        <v>1</v>
-      </c>
-      <c r="D11" s="58">
-        <v>0</v>
-      </c>
-      <c r="E11" s="58">
-        <v>0</v>
-      </c>
-      <c r="F11" s="58">
-        <v>0</v>
-      </c>
-      <c r="G11" s="57">
-        <v>1</v>
-      </c>
-      <c r="H11" s="58">
-        <v>1</v>
-      </c>
-      <c r="I11" s="59">
-        <v>1</v>
-      </c>
-      <c r="J11" s="59" t="str">
+      <c r="C11" s="56">
+        <v>1</v>
+      </c>
+      <c r="D11" s="56">
+        <v>0</v>
+      </c>
+      <c r="E11" s="56">
+        <v>0</v>
+      </c>
+      <c r="F11" s="56">
+        <v>0</v>
+      </c>
+      <c r="G11" s="55">
+        <v>1</v>
+      </c>
+      <c r="H11" s="56">
+        <v>1</v>
+      </c>
+      <c r="I11" s="57">
+        <v>1</v>
+      </c>
+      <c r="J11" s="57" t="str">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="49" t="str">
+      <c r="B12" s="47" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -4172,16 +4172,16 @@
       <c r="F12" s="25">
         <v>1</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="45">
         <v>1</v>
       </c>
       <c r="H12" s="25">
         <v>1</v>
       </c>
-      <c r="I12" s="48">
-        <v>0</v>
-      </c>
-      <c r="J12" s="48" t="str">
+      <c r="I12" s="46">
+        <v>0</v>
+      </c>
+      <c r="J12" s="46" t="str">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="49" t="str">
+      <c r="B13" s="47" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
@@ -4205,16 +4205,16 @@
       <c r="F13" s="25">
         <v>0</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="45">
         <v>1</v>
       </c>
       <c r="H13" s="25">
         <v>0</v>
       </c>
-      <c r="I13" s="48">
-        <v>1</v>
-      </c>
-      <c r="J13" s="48" t="str">
+      <c r="I13" s="46">
+        <v>1</v>
+      </c>
+      <c r="J13" s="46" t="str">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="49" t="str">
+      <c r="B14" s="47" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
@@ -4238,16 +4238,16 @@
       <c r="F14" s="25">
         <v>1</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="45">
         <v>1</v>
       </c>
       <c r="H14" s="25">
         <v>0</v>
       </c>
-      <c r="I14" s="48">
-        <v>0</v>
-      </c>
-      <c r="J14" s="48" t="str">
+      <c r="I14" s="46">
+        <v>0</v>
+      </c>
+      <c r="J14" s="46" t="str">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4255,7 +4255,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="49" t="str">
+      <c r="B15" s="47" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
@@ -4271,16 +4271,16 @@
       <c r="F15" s="25">
         <v>0</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="45">
         <v>0</v>
       </c>
       <c r="H15" s="25">
         <v>1</v>
       </c>
-      <c r="I15" s="48">
-        <v>1</v>
-      </c>
-      <c r="J15" s="48" t="str">
+      <c r="I15" s="46">
+        <v>1</v>
+      </c>
+      <c r="J15" s="46" t="str">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -4288,7 +4288,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="49" t="str">
+      <c r="B16" s="47" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
@@ -4304,16 +4304,16 @@
       <c r="F16" s="25">
         <v>1</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="45">
         <v>0</v>
       </c>
       <c r="H16" s="25">
         <v>1</v>
       </c>
-      <c r="I16" s="48">
-        <v>0</v>
-      </c>
-      <c r="J16" s="48" t="str">
+      <c r="I16" s="46">
+        <v>0</v>
+      </c>
+      <c r="J16" s="46" t="str">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="49" t="str">
+      <c r="B17" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
@@ -4337,16 +4337,16 @@
       <c r="F17" s="25">
         <v>0</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="45">
         <v>0</v>
       </c>
       <c r="H17" s="25">
         <v>0</v>
       </c>
-      <c r="I17" s="48">
-        <v>1</v>
-      </c>
-      <c r="J17" s="48" t="str">
+      <c r="I17" s="46">
+        <v>1</v>
+      </c>
+      <c r="J17" s="46" t="str">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4354,32 +4354,32 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="52" t="str">
+      <c r="B18" s="50" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="C18" s="54">
-        <v>1</v>
-      </c>
-      <c r="D18" s="54">
-        <v>1</v>
-      </c>
-      <c r="E18" s="54">
-        <v>1</v>
-      </c>
-      <c r="F18" s="54">
-        <v>1</v>
-      </c>
-      <c r="G18" s="53">
-        <v>0</v>
-      </c>
-      <c r="H18" s="54">
-        <v>0</v>
-      </c>
-      <c r="I18" s="55">
-        <v>0</v>
-      </c>
-      <c r="J18" s="55" t="str">
+      <c r="C18" s="52">
+        <v>1</v>
+      </c>
+      <c r="D18" s="52">
+        <v>1</v>
+      </c>
+      <c r="E18" s="52">
+        <v>1</v>
+      </c>
+      <c r="F18" s="52">
+        <v>1</v>
+      </c>
+      <c r="G18" s="51">
+        <v>0</v>
+      </c>
+      <c r="H18" s="52">
+        <v>0</v>
+      </c>
+      <c r="I18" s="53">
+        <v>0</v>
+      </c>
+      <c r="J18" s="53" t="str">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Working on Execute: PWM commutation experiments, current tracking, fixed I2C data corruption, etc.
git-svn-id: https://svn.media.mit.edu/r/biomech-ee/Code/flexsea_1_0@548 ca98db78-25f0-4961-890e-003d10304561
</commit_message>
<xml_diff>
--- a/execute/ref/pwm.xlsx
+++ b/execute/ref/pwm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Brushed" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
   <si>
     <t>PWM</t>
   </si>
@@ -151,17 +151,23 @@
     <t>Looking at Hall=1:</t>
   </si>
   <si>
-    <t>When both phases are 0, low side FETs need to be OFF. Otherwise we get heavy damping.</t>
+    <t>Original 2Q table from TI E2E:</t>
   </si>
   <si>
-    <t>Original 2Q table from TI E2E:</t>
+    <t>Modified 2Q table:</t>
+  </si>
+  <si>
+    <t>The only difference between the modified 2Q and 4Q tables is the complementary switching. Forcing Phase 2 to 0 will place the drive in Coast Mode rather than in Brake mode.</t>
+  </si>
+  <si>
+    <t>When both phases are 0, low side FETs need to be OFF. Otherwise we get heavy damping (aka motor braking).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +235,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -593,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,30 +776,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -793,8 +789,57 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1135,7 @@
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
@@ -1103,28 +1148,29 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -1148,7 +1194,7 @@
       <c r="K3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="70">
+      <c r="L3" s="62">
         <v>0</v>
       </c>
       <c r="M3" s="5">
@@ -1160,8 +1206,9 @@
       <c r="O3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -1188,17 +1235,18 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="M4" s="71">
-        <v>0</v>
-      </c>
-      <c r="N4" s="71">
-        <v>1</v>
-      </c>
-      <c r="O4" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M4" s="63">
+        <v>0</v>
+      </c>
+      <c r="N4" s="63">
+        <v>1</v>
+      </c>
+      <c r="O4" s="64">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
@@ -1234,16 +1282,17 @@
         <f t="shared" ref="M5:O5" si="1">NOT(NOT(M4))</f>
         <v>0</v>
       </c>
-      <c r="N5" s="11" t="b">
+      <c r="N5" s="69" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O5" s="12" t="b">
+      <c r="O5" s="70" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -1287,8 +1336,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
         <v>4</v>
@@ -1316,11 +1366,11 @@
       <c r="K7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="31" t="b">
+      <c r="L7" s="71" t="b">
         <f>NOT(L4)</f>
         <v>1</v>
       </c>
-      <c r="M7" s="13" t="b">
+      <c r="M7" s="15" t="b">
         <f t="shared" ref="M7:O7" si="5">NOT(M4)</f>
         <v>1</v>
       </c>
@@ -1332,8 +1382,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
         <v>5</v>
@@ -1377,8 +1428,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -1406,24 +1458,25 @@
       <c r="K9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="73" t="b">
+      <c r="L9" s="65" t="b">
         <f>_xlfn.XOR(L5,L6)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="73" t="b">
+      <c r="M9" s="65" t="b">
         <f t="shared" ref="M9" si="9">_xlfn.XOR(M5,M6)</f>
         <v>1</v>
       </c>
-      <c r="N9" s="73" t="b">
+      <c r="N9" s="65" t="b">
         <f>_xlfn.XOR(N5,N6)</f>
         <v>1</v>
       </c>
-      <c r="O9" s="74" t="b">
+      <c r="O9" s="66" t="b">
         <f>_xlfn.XOR(O5,O6)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="7" t="s">
         <v>7</v>
@@ -1451,24 +1504,25 @@
       <c r="K10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="75" t="b">
+      <c r="L10" s="21" t="b">
         <f>AND(L5,L6)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="75" t="b">
+      <c r="M10" s="21" t="b">
         <f t="shared" ref="M10" si="11">AND(M5,M6)</f>
         <v>0</v>
       </c>
-      <c r="N10" s="75" t="b">
+      <c r="N10" s="21" t="b">
         <f>AND(N5,N6)</f>
         <v>0</v>
       </c>
-      <c r="O10" s="76" t="b">
+      <c r="O10" s="22" t="b">
         <f>AND(O5,O6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -1496,24 +1550,25 @@
       <c r="K11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="75" t="b">
+      <c r="L11" s="67" t="b">
         <f>_xlfn.XOR(L7,L8)</f>
         <v>1</v>
       </c>
-      <c r="M11" s="75" t="b">
+      <c r="M11" s="67" t="b">
         <f t="shared" ref="M11" si="13">_xlfn.XOR(M7,M8)</f>
         <v>1</v>
       </c>
-      <c r="N11" s="75" t="b">
+      <c r="N11" s="67" t="b">
         <f>_xlfn.XOR(N7,N8)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="76" t="b">
+      <c r="O11" s="68" t="b">
         <f>_xlfn.XOR(O7,O8)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1541,24 +1596,25 @@
       <c r="K12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="77" t="b">
+      <c r="L12" s="23" t="b">
         <f>AND(L7,L8)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="77" t="b">
+      <c r="M12" s="23" t="b">
         <f t="shared" ref="M12" si="15">AND(M7,M8)</f>
         <v>0</v>
       </c>
-      <c r="N12" s="77" t="b">
+      <c r="N12" s="23" t="b">
         <f>AND(N7,N8)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="78" t="b">
+      <c r="O12" s="24" t="b">
         <f>AND(O7,O8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
         <v>12</v>
@@ -1583,8 +1639,14 @@
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
       <c r="J13" s="21"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="7" t="s">
         <v>13</v>
@@ -1609,8 +1671,14 @@
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="21"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="26"/>
@@ -1626,8 +1694,9 @@
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="27" t="s">
         <v>9</v>
@@ -1641,14 +1710,15 @@
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="27" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
       <c r="O16" s="27"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
         <v>0</v>
@@ -1672,7 +1742,7 @@
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="62">
         <v>0</v>
       </c>
       <c r="M17" s="5">
@@ -1684,8 +1754,9 @@
       <c r="O17" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="7" t="s">
         <v>1</v>
@@ -1709,7 +1780,7 @@
       <c r="K18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="29">
         <v>0</v>
       </c>
       <c r="M18" s="8">
@@ -1721,8 +1792,9 @@
       <c r="O18" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="29" t="s">
         <v>2</v>
@@ -1748,26 +1820,27 @@
       <c r="I19" s="26"/>
       <c r="J19" s="13"/>
       <c r="K19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="30" t="b">
+        <v>4</v>
+      </c>
+      <c r="L19" s="74" t="b">
         <f>AND(NOT(L18),L17)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="11" t="b">
-        <f t="shared" ref="M19" si="19">AND(NOT(M18),M17)</f>
-        <v>1</v>
-      </c>
-      <c r="N19" s="11" t="b">
-        <f>AND(NOT(N18),N17)</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="12" t="b">
-        <f>AND(NOT(O18),O17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M19" s="75" t="b">
+        <f t="shared" ref="M19:O19" si="19">AND(NOT(M18),M17)</f>
+        <v>1</v>
+      </c>
+      <c r="N19" s="72" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="73" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="29" t="s">
         <v>3</v>
@@ -1793,26 +1866,27 @@
       <c r="I20" s="26"/>
       <c r="J20" s="13"/>
       <c r="K20" s="29" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L20" s="31" t="b">
-        <f>AND(L17,L18)</f>
+        <f>NOT(NOT(L18))</f>
         <v>0</v>
       </c>
       <c r="M20" s="13" t="b">
-        <f t="shared" ref="M20" si="21">AND(M17,M18)</f>
+        <f t="shared" ref="M20:O20" si="21">NOT(NOT(M18))</f>
         <v>0</v>
       </c>
       <c r="N20" s="13" t="b">
-        <f>AND(N17,N18)</f>
-        <v>0</v>
+        <f t="shared" si="21"/>
+        <v>1</v>
       </c>
       <c r="O20" s="14" t="b">
-        <f>AND(O17,O18)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="29" t="s">
         <v>4</v>
@@ -1838,26 +1912,27 @@
       <c r="I21" s="26"/>
       <c r="J21" s="32"/>
       <c r="K21" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="31" t="b">
-        <f>L19</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="13" t="b">
-        <f t="shared" ref="M21" si="23">M19</f>
-        <v>1</v>
-      </c>
-      <c r="N21" s="32" t="b">
-        <f>N19</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="33" t="b">
-        <f>O19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="L21" s="34" t="b">
+        <f>AND(L17,L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="32" t="b">
+        <f t="shared" ref="M21:O21" si="23">AND(M17,M18)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="76" t="b">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="77" t="b">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="29" t="s">
         <v>5</v>
@@ -1882,27 +1957,28 @@
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
       <c r="J22" s="13"/>
-      <c r="K22" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="L22" s="31" t="b">
-        <f>NOT(L19)</f>
-        <v>1</v>
-      </c>
-      <c r="M22" s="13" t="b">
-        <f t="shared" ref="M22" si="25">NOT(M19)</f>
-        <v>0</v>
-      </c>
-      <c r="N22" s="13" t="b">
-        <f>NOT(N19)</f>
-        <v>1</v>
-      </c>
-      <c r="O22" s="14" t="b">
-        <f>NOT(O19)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="36" t="b">
+        <f>NOT(L18)</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="17" t="b">
+        <f t="shared" ref="M22:O22" si="25">NOT(M18)</f>
+        <v>1</v>
+      </c>
+      <c r="N22" s="17" t="b">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="18" t="b">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="29" t="s">
         <v>6</v>
@@ -1927,27 +2003,28 @@
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" s="34" t="b">
-        <f>(L20)</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="32" t="b">
-        <f t="shared" ref="M23" si="27">(M20)</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="13" t="b">
-        <f>(N20)</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="14" t="b">
-        <f>(O20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="67" t="b">
+        <f>_xlfn.XOR(L19,L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="67" t="b">
+        <f t="shared" ref="M23" si="27">_xlfn.XOR(M19,M20)</f>
+        <v>1</v>
+      </c>
+      <c r="N23" s="67" t="b">
+        <f>_xlfn.XOR(N19,N20)</f>
+        <v>1</v>
+      </c>
+      <c r="O23" s="68" t="b">
+        <f>_xlfn.XOR(O19,O20)</f>
+        <v>1</v>
+      </c>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="35" t="s">
         <v>7</v>
@@ -1972,27 +2049,28 @@
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="L24" s="36" t="b">
-        <f>NOT(L20)</f>
-        <v>1</v>
-      </c>
-      <c r="M24" s="17" t="b">
-        <f t="shared" ref="M24" si="29">NOT(M20)</f>
-        <v>1</v>
-      </c>
-      <c r="N24" s="17" t="b">
-        <f>NOT(N20)</f>
-        <v>1</v>
-      </c>
-      <c r="O24" s="18" t="b">
-        <f>NOT(O20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="21" t="b">
+        <f>AND(L19,L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="21" t="b">
+        <f t="shared" ref="M24" si="29">AND(M19,M20)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="21" t="b">
+        <f>AND(N19,N20)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="22" t="b">
+        <f>AND(O19,O20)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="39" t="s">
         <v>17</v>
@@ -2013,23 +2091,28 @@
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="N25" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="O25" s="38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="67" t="b">
+        <f>_xlfn.XOR(L21,L22)</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="67" t="b">
+        <f t="shared" ref="M25" si="30">_xlfn.XOR(M21,M22)</f>
+        <v>1</v>
+      </c>
+      <c r="N25" s="67" t="b">
+        <f>_xlfn.XOR(N21,N22)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="68" t="b">
+        <f>_xlfn.XOR(O21,O22)</f>
+        <v>1</v>
+      </c>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="10" t="s">
         <v>10</v>
@@ -2054,27 +2137,28 @@
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L26" s="21" t="b">
-        <f>_xlfn.XOR(L21,L22)</f>
-        <v>1</v>
-      </c>
-      <c r="M26" s="21" t="b">
-        <f>_xlfn.XOR(M21,M22)</f>
-        <v>1</v>
-      </c>
-      <c r="N26" s="21" t="b">
-        <f>_xlfn.XOR(N21,N22)</f>
-        <v>1</v>
-      </c>
-      <c r="O26" s="22" t="b">
-        <f>_xlfn.XOR(O21,O22)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="23" t="b">
+        <f>AND(L21,L22)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="23" t="b">
+        <f t="shared" ref="M26" si="31">AND(M21,M22)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="23" t="b">
+        <f>AND(N21,N22)</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="24" t="b">
+        <f>AND(O21,O22)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="10" t="s">
         <v>11</v>
@@ -2099,27 +2183,14 @@
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="21" t="b">
-        <f>AND(L21,L22)</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="21" t="b">
-        <f>AND(M21,M22)</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="21" t="b">
-        <f>AND(N21,N22)</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="22" t="b">
-        <f>AND(O21,O22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K27" s="8"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="10" t="s">
         <v>12</v>
@@ -2144,27 +2215,16 @@
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="21"/>
-      <c r="K28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L28" s="21" t="b">
-        <f>_xlfn.XOR(L23,L24)</f>
-        <v>1</v>
-      </c>
-      <c r="M28" s="21" t="b">
-        <f>_xlfn.XOR(M23,M24)</f>
-        <v>1</v>
-      </c>
-      <c r="N28" s="21" t="b">
-        <f>_xlfn.XOR(N23,N24)</f>
-        <v>1</v>
-      </c>
-      <c r="O28" s="22" t="b">
-        <f>_xlfn.XOR(O23,O24)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="80"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="7" t="s">
         <v>13</v>
@@ -2189,27 +2249,14 @@
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="21"/>
-      <c r="K29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L29" s="23" t="b">
-        <f>AND(L23,L24)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="23" t="b">
-        <f>AND(M23,M24)</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="23" t="b">
-        <f>AND(N23,N24)</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="24" t="b">
-        <f>AND(O23,O24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
@@ -2220,9 +2267,14 @@
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="80"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
@@ -2234,12 +2286,18 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:O2"/>
+    <mergeCell ref="K28:O30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2250,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,44 +2365,44 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="U2" s="68" t="s">
+      <c r="U2" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="68"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="68"/>
-      <c r="AH2" s="68"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -2405,23 +2463,23 @@
       <c r="S4" s="2"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="65" t="s">
+      <c r="W4" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="65" t="s">
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="67"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="82"/>
+      <c r="AE4" s="82"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="82"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="83"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="2"/>
     </row>
@@ -2564,19 +2622,19 @@
       <c r="J6" s="25">
         <v>0</v>
       </c>
-      <c r="K6" s="62">
-        <v>1</v>
-      </c>
-      <c r="L6" s="62">
-        <v>0</v>
-      </c>
-      <c r="M6" s="62">
-        <v>0</v>
-      </c>
-      <c r="N6" s="62">
-        <v>0</v>
-      </c>
-      <c r="O6" s="62">
+      <c r="K6" s="25">
+        <v>1</v>
+      </c>
+      <c r="L6" s="25">
+        <v>0</v>
+      </c>
+      <c r="M6" s="25">
+        <v>0</v>
+      </c>
+      <c r="N6" s="25">
+        <v>0</v>
+      </c>
+      <c r="O6" s="25">
         <f>E6</f>
         <v>0</v>
       </c>
@@ -2680,21 +2738,21 @@
       <c r="J7" s="25">
         <v>0</v>
       </c>
-      <c r="K7" s="62">
-        <v>0</v>
-      </c>
-      <c r="L7" s="62">
-        <v>0</v>
-      </c>
-      <c r="M7" s="62">
+      <c r="K7" s="25">
+        <v>0</v>
+      </c>
+      <c r="L7" s="25">
+        <v>0</v>
+      </c>
+      <c r="M7" s="25">
         <f>E7</f>
         <v>0</v>
       </c>
-      <c r="N7" s="62">
+      <c r="N7" s="25">
         <f>D7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="62">
+      <c r="O7" s="25">
         <v>1</v>
       </c>
       <c r="P7" s="46">
@@ -2799,21 +2857,21 @@
       <c r="J8" s="25">
         <v>0</v>
       </c>
-      <c r="K8" s="62">
-        <v>1</v>
-      </c>
-      <c r="L8" s="62">
-        <v>0</v>
-      </c>
-      <c r="M8" s="62">
+      <c r="K8" s="25">
+        <v>1</v>
+      </c>
+      <c r="L8" s="25">
+        <v>0</v>
+      </c>
+      <c r="M8" s="25">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="N8" s="62">
+      <c r="N8" s="25">
         <f>D8</f>
         <v>0</v>
       </c>
-      <c r="O8" s="62">
+      <c r="O8" s="25">
         <v>0</v>
       </c>
       <c r="P8" s="46">
@@ -2918,21 +2976,21 @@
       <c r="J9" s="25">
         <v>1</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="25">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="L9" s="62">
+      <c r="L9" s="25">
         <f>D9</f>
         <v>0</v>
       </c>
-      <c r="M9" s="62">
-        <v>1</v>
-      </c>
-      <c r="N9" s="62">
-        <v>0</v>
-      </c>
-      <c r="O9" s="62">
+      <c r="M9" s="25">
+        <v>1</v>
+      </c>
+      <c r="N9" s="25">
+        <v>0</v>
+      </c>
+      <c r="O9" s="25">
         <v>0</v>
       </c>
       <c r="P9" s="46">
@@ -3035,19 +3093,19 @@
       <c r="J10" s="25">
         <v>1</v>
       </c>
-      <c r="K10" s="62">
-        <v>0</v>
-      </c>
-      <c r="L10" s="62">
-        <v>0</v>
-      </c>
-      <c r="M10" s="62">
-        <v>1</v>
-      </c>
-      <c r="N10" s="62">
-        <v>0</v>
-      </c>
-      <c r="O10" s="62">
+      <c r="K10" s="25">
+        <v>0</v>
+      </c>
+      <c r="L10" s="25">
+        <v>0</v>
+      </c>
+      <c r="M10" s="25">
+        <v>1</v>
+      </c>
+      <c r="N10" s="25">
+        <v>0</v>
+      </c>
+      <c r="O10" s="25">
         <f>E10</f>
         <v>0</v>
       </c>
@@ -3095,21 +3153,21 @@
       <c r="J11" s="25">
         <v>0</v>
       </c>
-      <c r="K11" s="62">
+      <c r="K11" s="25">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="25">
         <f>D11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="62">
-        <v>0</v>
-      </c>
-      <c r="N11" s="62">
-        <v>0</v>
-      </c>
-      <c r="O11" s="62">
+      <c r="M11" s="25">
+        <v>0</v>
+      </c>
+      <c r="N11" s="25">
+        <v>0</v>
+      </c>
+      <c r="O11" s="25">
         <v>1</v>
       </c>
       <c r="P11" s="46">
@@ -3182,22 +3240,22 @@
         <v>0</v>
       </c>
       <c r="S12" s="2"/>
-      <c r="U12" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="V12" s="68"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="68"/>
-      <c r="Y12" s="68"/>
-      <c r="Z12" s="68"/>
-      <c r="AA12" s="68"/>
-      <c r="AB12" s="68"/>
-      <c r="AC12" s="68"/>
-      <c r="AD12" s="68"/>
-      <c r="AE12" s="68"/>
-      <c r="AF12" s="68"/>
-      <c r="AG12" s="68"/>
-      <c r="AH12" s="68"/>
+      <c r="U12" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="V12" s="84"/>
+      <c r="W12" s="84"/>
+      <c r="X12" s="84"/>
+      <c r="Y12" s="84"/>
+      <c r="Z12" s="84"/>
+      <c r="AA12" s="84"/>
+      <c r="AB12" s="84"/>
+      <c r="AC12" s="84"/>
+      <c r="AD12" s="84"/>
+      <c r="AE12" s="84"/>
+      <c r="AF12" s="84"/>
+      <c r="AG12" s="84"/>
+      <c r="AH12" s="84"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>

</xml_diff>

<commit_message>
Execute: use Brake and not Coast.
git-svn-id: https://svn.media.mit.edu/r/biomech-ee/Code/flexsea_1_0@567 ca98db78-25f0-4961-890e-003d10304561
</commit_message>
<xml_diff>
--- a/execute/ref/pwm.xlsx
+++ b/execute/ref/pwm.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
   <si>
     <t>PWM</t>
   </si>
@@ -162,6 +162,12 @@
   <si>
     <t>When both phases are 0, low side FETs need to be OFF. Otherwise we get heavy damping (aka motor braking).</t>
   </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
 </sst>
 </file>
 
@@ -250,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +281,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -613,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,6 +850,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2309,7 +2327,7 @@
   <dimension ref="A1:AL37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:O11"/>
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,8 +2378,12 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -3495,7 +3517,7 @@
       </c>
       <c r="S16" s="2"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3555,7 +3577,7 @@
       </c>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3615,7 +3637,7 @@
       </c>
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3675,7 +3697,7 @@
       </c>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3733,7 +3755,7 @@
       </c>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="44" t="str">
         <f t="shared" si="0"/>
@@ -3790,8 +3812,62 @@
         <v>0</v>
       </c>
       <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V21" s="44" t="str">
+        <f t="shared" ref="V21:V28" si="6">DEC2HEX(1*AB21+2*AA21+4*Z21+8*Y21+16*X21)</f>
+        <v>10</v>
+      </c>
+      <c r="W21" s="44">
+        <v>0</v>
+      </c>
+      <c r="X21" s="56">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="57">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="57">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="56">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="44" t="str">
+        <f>DEC2HEX(1*AI21+2*AJ21+4*AG21+8*AH21+16*AE21+32*AF21+64*AD21+128*AC21)</f>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="48" t="b">
+        <f>OR(AND(AF21,AE21), AND(AH21,AG21), AND(AJ21,AI21))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3821,23 +3897,23 @@
       <c r="J22" s="25">
         <v>0</v>
       </c>
-      <c r="K22" s="25">
-        <v>1</v>
-      </c>
-      <c r="L22" s="25">
-        <v>0</v>
-      </c>
-      <c r="M22" s="25">
-        <v>0</v>
-      </c>
-      <c r="N22" s="25">
-        <v>0</v>
-      </c>
-      <c r="O22" s="25">
+      <c r="K22" s="86">
+        <v>1</v>
+      </c>
+      <c r="L22" s="86">
+        <v>0</v>
+      </c>
+      <c r="M22" s="86">
+        <v>0</v>
+      </c>
+      <c r="N22" s="86">
+        <v>0</v>
+      </c>
+      <c r="O22" s="86">
         <f>E22</f>
         <v>0</v>
       </c>
-      <c r="P22" s="46">
+      <c r="P22" s="87">
         <f>D22</f>
         <v>1</v>
       </c>
@@ -3850,8 +3926,64 @@
         <v>0</v>
       </c>
       <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V22" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="W22" s="47">
+        <v>1</v>
+      </c>
+      <c r="X22" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="46">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="25">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="86">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="86">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="86">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="87">
+        <f>X22</f>
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="86">
+        <f>Y22</f>
+        <v>0</v>
+      </c>
+      <c r="AK22" s="47" t="str">
+        <f>DEC2HEX(1*AI22+2*AJ22+4*AG22+8*AH22+16*AE22+32*AF22+64*AD22+128*AC22)</f>
+        <v>A1</v>
+      </c>
+      <c r="AL22" s="49" t="b">
+        <f>OR(AND(AF22,AE22), AND(AH22,AG22), AND(AJ22,AI22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3881,24 +4013,24 @@
       <c r="J23" s="25">
         <v>0</v>
       </c>
-      <c r="K23" s="25">
-        <v>0</v>
-      </c>
-      <c r="L23" s="25">
-        <v>0</v>
-      </c>
-      <c r="M23" s="25">
+      <c r="K23" s="86">
+        <v>0</v>
+      </c>
+      <c r="L23" s="86">
+        <v>0</v>
+      </c>
+      <c r="M23" s="86">
         <f>E23</f>
         <v>0</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="86">
         <f>D23</f>
         <v>1</v>
       </c>
-      <c r="O23" s="25">
-        <v>1</v>
-      </c>
-      <c r="P23" s="46">
+      <c r="O23" s="86">
+        <v>1</v>
+      </c>
+      <c r="P23" s="87">
         <v>0</v>
       </c>
       <c r="Q23" s="47" t="str">
@@ -3910,8 +4042,64 @@
         <v>0</v>
       </c>
       <c r="S23" s="2"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V23" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="W23" s="47">
+        <v>2</v>
+      </c>
+      <c r="X23" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="25">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="46">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="86">
+        <f>X23</f>
+        <v>1</v>
+      </c>
+      <c r="AH23" s="86">
+        <f>Y23</f>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="86">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="47" t="str">
+        <f>DEC2HEX(1*AI23+2*AJ23+4*AG23+8*AH23+16*AE23+32*AF23+64*AD23+128*AC23)</f>
+        <v>6</v>
+      </c>
+      <c r="AL23" s="49" t="b">
+        <f>OR(AND(AF23,AE23), AND(AH23,AG23), AND(AJ23,AI23))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="47" t="str">
         <f t="shared" si="0"/>
@@ -3941,24 +4129,24 @@
       <c r="J24" s="25">
         <v>0</v>
       </c>
-      <c r="K24" s="25">
-        <v>1</v>
-      </c>
-      <c r="L24" s="25">
-        <v>0</v>
-      </c>
-      <c r="M24" s="25">
+      <c r="K24" s="86">
+        <v>1</v>
+      </c>
+      <c r="L24" s="86">
+        <v>0</v>
+      </c>
+      <c r="M24" s="86">
         <f>E24</f>
         <v>0</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="86">
         <f>D24</f>
         <v>1</v>
       </c>
-      <c r="O24" s="25">
-        <v>0</v>
-      </c>
-      <c r="P24" s="46">
+      <c r="O24" s="86">
+        <v>0</v>
+      </c>
+      <c r="P24" s="87">
         <v>0</v>
       </c>
       <c r="Q24" s="47" t="str">
@@ -3970,8 +4158,64 @@
         <v>0</v>
       </c>
       <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V24" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="W24" s="47">
+        <v>3</v>
+      </c>
+      <c r="X24" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="25">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="46">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="25">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="86">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="86">
+        <f>X24</f>
+        <v>1</v>
+      </c>
+      <c r="AH24" s="86">
+        <f>Y24</f>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="86">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="47" t="str">
+        <f>DEC2HEX(1*AI24+2*AJ24+4*AG24+8*AH24+16*AE24+32*AF24+64*AD24+128*AC24)</f>
+        <v>A4</v>
+      </c>
+      <c r="AL24" s="49" t="b">
+        <f>OR(AND(AF24,AE24), AND(AH24,AG24), AND(AJ24,AI24))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="47" t="str">
         <f t="shared" si="0"/>
@@ -4001,24 +4245,24 @@
       <c r="J25" s="25">
         <v>1</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="86">
         <f>E25</f>
         <v>0</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="86">
         <f>D25</f>
         <v>1</v>
       </c>
-      <c r="M25" s="25">
-        <v>1</v>
-      </c>
-      <c r="N25" s="25">
-        <v>0</v>
-      </c>
-      <c r="O25" s="25">
-        <v>0</v>
-      </c>
-      <c r="P25" s="46">
+      <c r="M25" s="86">
+        <v>1</v>
+      </c>
+      <c r="N25" s="86">
+        <v>0</v>
+      </c>
+      <c r="O25" s="86">
+        <v>0</v>
+      </c>
+      <c r="P25" s="87">
         <v>0</v>
       </c>
       <c r="Q25" s="47" t="str">
@@ -4030,8 +4274,64 @@
         <v>0</v>
       </c>
       <c r="S25" s="2"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V25" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="W25" s="47">
+        <v>4</v>
+      </c>
+      <c r="X25" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="46">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="25">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="86">
+        <f>X25</f>
+        <v>1</v>
+      </c>
+      <c r="AF25" s="86">
+        <f>Y25</f>
+        <v>0</v>
+      </c>
+      <c r="AG25" s="86">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="86">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="86">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="47" t="str">
+        <f>DEC2HEX(1*AI25+2*AJ25+4*AG25+8*AH25+16*AE25+32*AF25+64*AD25+128*AC25)</f>
+        <v>58</v>
+      </c>
+      <c r="AL25" s="49" t="b">
+        <f>OR(AND(AF25,AE25), AND(AH25,AG25), AND(AJ25,AI25))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="47" t="str">
         <f t="shared" si="0"/>
@@ -4061,23 +4361,23 @@
       <c r="J26" s="25">
         <v>1</v>
       </c>
-      <c r="K26" s="25">
-        <v>0</v>
-      </c>
-      <c r="L26" s="25">
-        <v>0</v>
-      </c>
-      <c r="M26" s="25">
-        <v>1</v>
-      </c>
-      <c r="N26" s="25">
-        <v>0</v>
-      </c>
-      <c r="O26" s="25">
+      <c r="K26" s="86">
+        <v>0</v>
+      </c>
+      <c r="L26" s="86">
+        <v>0</v>
+      </c>
+      <c r="M26" s="86">
+        <v>1</v>
+      </c>
+      <c r="N26" s="86">
+        <v>0</v>
+      </c>
+      <c r="O26" s="86">
         <f>E26</f>
         <v>0</v>
       </c>
-      <c r="P26" s="46">
+      <c r="P26" s="87">
         <f>D26</f>
         <v>1</v>
       </c>
@@ -4090,8 +4390,64 @@
         <v>0</v>
       </c>
       <c r="S26" s="2"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V26" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="W26" s="47">
+        <v>5</v>
+      </c>
+      <c r="X26" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="46">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="25">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="86">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="86">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="87">
+        <f>X26</f>
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="86">
+        <f>Y26</f>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="47" t="str">
+        <f>DEC2HEX(1*AI26+2*AJ26+4*AG26+8*AH26+16*AE26+32*AF26+64*AD26+128*AC26)</f>
+        <v>49</v>
+      </c>
+      <c r="AL26" s="49" t="b">
+        <f>OR(AND(AF26,AE26), AND(AH26,AG26), AND(AJ26,AI26))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="47" t="str">
         <f t="shared" si="0"/>
@@ -4121,24 +4477,24 @@
       <c r="J27" s="25">
         <v>0</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="86">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="86">
         <f>D27</f>
         <v>1</v>
       </c>
-      <c r="M27" s="25">
-        <v>0</v>
-      </c>
-      <c r="N27" s="25">
-        <v>0</v>
-      </c>
-      <c r="O27" s="25">
-        <v>1</v>
-      </c>
-      <c r="P27" s="46">
+      <c r="M27" s="86">
+        <v>0</v>
+      </c>
+      <c r="N27" s="86">
+        <v>0</v>
+      </c>
+      <c r="O27" s="86">
+        <v>1</v>
+      </c>
+      <c r="P27" s="87">
         <v>0</v>
       </c>
       <c r="Q27" s="47" t="str">
@@ -4150,8 +4506,64 @@
         <v>0</v>
       </c>
       <c r="S27" s="2"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V27" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="W27" s="47">
+        <v>6</v>
+      </c>
+      <c r="X27" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="25">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="46">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="25">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="86">
+        <f>X27</f>
+        <v>1</v>
+      </c>
+      <c r="AF27" s="86">
+        <f>Y27</f>
+        <v>0</v>
+      </c>
+      <c r="AG27" s="86">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="86">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="86">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="47" t="str">
+        <f>DEC2HEX(1*AI27+2*AJ27+4*AG27+8*AH27+16*AE27+32*AF27+64*AD27+128*AC27)</f>
+        <v>12</v>
+      </c>
+      <c r="AL27" s="49" t="b">
+        <f>OR(AND(AF27,AE27), AND(AH27,AG27), AND(AJ27,AI27))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="50" t="str">
         <f t="shared" si="0"/>
@@ -4208,8 +4620,62 @@
         <v>0</v>
       </c>
       <c r="S28" s="2"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V28" s="50" t="str">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="W28" s="50">
+        <v>7</v>
+      </c>
+      <c r="X28" s="52">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="52">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="52">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="53">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="53">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="52">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="50" t="str">
+        <f>DEC2HEX(1*AI28+2*AJ28+4*AG28+8*AH28+16*AE28+32*AF28+64*AD28+128*AC28)</f>
+        <v>0</v>
+      </c>
+      <c r="AL28" s="54" t="b">
+        <f>OR(AND(AF28,AE28), AND(AH28,AG28), AND(AJ28,AI28))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="44" t="str">
         <f t="shared" si="0"/>
@@ -4267,7 +4733,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="47" t="str">
         <f t="shared" si="0"/>
@@ -4325,7 +4791,7 @@
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="47" t="str">
         <f t="shared" si="0"/>
@@ -4383,7 +4849,7 @@
       </c>
       <c r="S31" s="2"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="47" t="str">
         <f t="shared" si="0"/>

</xml_diff>